<commit_message>
refactored code for dynamic reports
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,12 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Practice Frameworks\MySeleniumFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD9257A6-8000-4CED-8D34-01B7A030409B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06203ACD-B854-4D1C-8318-BA835F19911E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="runData" sheetId="1" r:id="rId1"/>
+    <sheet name="RUNMANAGER" sheetId="2" r:id="rId1"/>
+    <sheet name="testData" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
   <si>
     <t>testcasename</t>
   </si>
@@ -39,24 +40,12 @@
     <t>assertion value</t>
   </si>
   <si>
-    <t>verifyHomePage</t>
-  </si>
-  <si>
-    <t>login</t>
-  </si>
-  <si>
-    <t>invalidLogin</t>
-  </si>
-  <si>
     <t>Admin</t>
   </si>
   <si>
     <t>admin123</t>
   </si>
   <si>
-    <t>manda user</t>
-  </si>
-  <si>
     <t>Admin1</t>
   </si>
   <si>
@@ -66,9 +55,6 @@
     <t>Invalid credentials</t>
   </si>
   <si>
-    <t>verifyFooterText</t>
-  </si>
-  <si>
     <t>OrangeHRM OS 5.7</t>
   </si>
   <si>
@@ -85,14 +71,49 @@
   </si>
   <si>
     <t>Dashboard</t>
+  </si>
+  <si>
+    <t>loginLogoutTest</t>
+  </si>
+  <si>
+    <t>invalidLoginTest</t>
+  </si>
+  <si>
+    <t>verifyHomePageTest</t>
+  </si>
+  <si>
+    <t>verifyFooterTextTest</t>
+  </si>
+  <si>
+    <t>OrangeHRM</t>
+  </si>
+  <si>
+    <t>priority</t>
+  </si>
+  <si>
+    <t>count</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>OrangeHRM123</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
@@ -108,7 +129,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -116,12 +137,30 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -401,11 +440,103 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6CA994-C3F9-4105-BBBF-EBA8078D124E}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="D2" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="D3" s="2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="2"/>
+      <c r="D4" s="2">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="2"/>
+      <c r="D5" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="2"/>
+      <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1:H14"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,105 +548,122 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+      <c r="B2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B2" t="s">
+      <c r="D2" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A4" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B4" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D4" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E4" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A5" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C5" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E5" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A6" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B6" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D6" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B3" t="s">
-        <v>10</v>
-      </c>
-      <c r="C3" t="s">
-        <v>11</v>
-      </c>
-      <c r="D3" t="s">
+      <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="E3" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="B4" t="s">
-        <v>7</v>
-      </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4" t="s">
-        <v>7</v>
-      </c>
-      <c r="E4" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>13</v>
-      </c>
-      <c r="B5" t="s">
-        <v>7</v>
-      </c>
-      <c r="C5" t="s">
-        <v>8</v>
-      </c>
-      <c r="D5" t="s">
+      <c r="C7" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D7" s="2" t="s">
         <v>14</v>
       </c>
-      <c r="E5" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>18</v>
-      </c>
-      <c r="B6" t="s">
-        <v>7</v>
-      </c>
-      <c r="C6" t="s">
-        <v>8</v>
-      </c>
-      <c r="D6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E6" t="s">
-        <v>16</v>
+      <c r="E7" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added listeners and dataprovider enhancements
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Practice Frameworks\MySeleniumFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{06203ACD-B854-4D1C-8318-BA835F19911E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB61523-F6D2-4696-A223-1AAFAB99F8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="RUNMANAGER" sheetId="2" r:id="rId1"/>
-    <sheet name="testData" sheetId="1" r:id="rId2"/>
+    <sheet name="TESTDATA" sheetId="1" r:id="rId2"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
   <si>
     <t>testcasename</t>
   </si>
@@ -98,6 +98,36 @@
   </si>
   <si>
     <t>OrangeHRM123</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>To verify if user can successfully login and logout</t>
+  </si>
+  <si>
+    <t>To verify if error is prompted on invalid login</t>
+  </si>
+  <si>
+    <t>To verify user is able to access Admin page</t>
+  </si>
+  <si>
+    <t>To verify footer is present</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>Admin123</t>
   </si>
 </sst>
 </file>
@@ -441,88 +471,117 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0A6CA994-C3F9-4105-BBBF-EBA8078D124E}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C5" sqref="C5"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="51.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="D1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="E1" s="1" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C2" s="2"/>
-      <c r="D2" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>16</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="2"/>
-      <c r="D3" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>26</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>17</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="2"/>
-      <c r="D4" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>27</v>
+      </c>
+      <c r="C4" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B5" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C5" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C5" s="2"/>
       <c r="D5" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="3" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C6" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="2"/>
       <c r="D6" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>22</v>
       </c>
     </row>
@@ -533,10 +592,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E7"/>
+  <dimension ref="A1:E8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D18" sqref="D18"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -666,6 +725,23 @@
         <v>11</v>
       </c>
     </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B8" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="C8" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="E8" s="2" t="s">
+        <v>11</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
added cross browser capability
</commit_message>
<xml_diff>
--- a/src/test/resources/testdata.xlsx
+++ b/src/test/resources/testdata.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Practice Frameworks\MySeleniumFramework\src\test\resources\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6CB61523-F6D2-4696-A223-1AAFAB99F8F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B2FE86B2-1D56-4962-831D-44423D87FA68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3855" yWindow="3855" windowWidth="21600" windowHeight="11295" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="34">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="38">
   <si>
     <t>testcasename</t>
   </si>
@@ -128,6 +128,18 @@
   </si>
   <si>
     <t>Admin123</t>
+  </si>
+  <si>
+    <t>browser</t>
+  </si>
+  <si>
+    <t>chrome</t>
+  </si>
+  <si>
+    <t>firefox</t>
+  </si>
+  <si>
+    <t>edge</t>
   </si>
 </sst>
 </file>
@@ -186,11 +198,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -474,7 +487,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -514,7 +527,7 @@
         <v>29</v>
       </c>
       <c r="E2" s="3" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -559,13 +572,13 @@
         <v>28</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>32</v>
       </c>
       <c r="E5" s="3" t="s">
-        <v>22</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
@@ -592,10 +605,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E8"/>
+  <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -606,7 +619,7 @@
     <col min="4" max="4" width="18.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -622,8 +635,11 @@
       <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F1" s="4" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -639,8 +655,11 @@
       <c r="E2" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F2" s="2" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>15</v>
       </c>
@@ -656,8 +675,11 @@
       <c r="E3" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F3" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>16</v>
       </c>
@@ -673,8 +695,11 @@
       <c r="E4" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F4" s="3" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>17</v>
       </c>
@@ -690,8 +715,11 @@
       <c r="E5" s="2" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F5" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>18</v>
       </c>
@@ -707,8 +735,11 @@
       <c r="E6" s="2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F6" s="2" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>13</v>
       </c>
@@ -722,10 +753,13 @@
         <v>14</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="F7" s="2" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>15</v>
       </c>
@@ -739,7 +773,10 @@
         <v>19</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>11</v>
+        <v>12</v>
+      </c>
+      <c r="F8" s="2" t="s">
+        <v>35</v>
       </c>
     </row>
   </sheetData>

</xml_diff>